<commit_message>
Add csv file with DNA/retrotransposon classification data, add references to final ranking excel file
</commit_message>
<xml_diff>
--- a/17_RepeatAge/out_cleanAgeRank/agerank_summary.xlsx
+++ b/17_RepeatAge/out_cleanAgeRank/agerank_summary.xlsx
@@ -1,25 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ltamon/DPhil/GenomicContactDynamics/7_RepeatAge/out_ageRank/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ltamon/SahakyanLab/GenomicContactDynamics/17_RepeatAge/out_cleanAgeRank/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB02942-C1D4-444C-9FC8-786DC6AE9BD4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5387D861-E6CC-C94D-A290-B704E040E11F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" firstSheet="1" activeTab="1" xr2:uid="{17B95E1A-9E60-0046-9EEE-407ED6BA80A9}"/>
+    <workbookView xWindow="700" yWindow="0" windowWidth="32900" windowHeight="21000" firstSheet="1" activeTab="2" xr2:uid="{17B95E1A-9E60-0046-9EEE-407ED6BA80A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Giordano364" sheetId="1" r:id="rId1"/>
     <sheet name="GiorPubl372" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="5" r:id="rId3"/>
-    <sheet name="Publ105" sheetId="3" r:id="rId4"/>
-    <sheet name="Reference" sheetId="4" r:id="rId5"/>
-    <sheet name="orderPbasedonG" sheetId="6" r:id="rId6"/>
-    <sheet name="orderPublished_basedonGiordano" sheetId="7" r:id="rId7"/>
+    <sheet name="Publ105" sheetId="3" r:id="rId3"/>
+    <sheet name="Reference" sheetId="4" r:id="rId4"/>
+    <sheet name="orderPbasedonG" sheetId="6" r:id="rId5"/>
+    <sheet name="orderPublished_basedonGiordano" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +28,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1516,7 +1520,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1804,7 +1808,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -9129,8 +9133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4948C8A8-9E75-8F4E-A339-74B100808E07}">
   <dimension ref="A1:F373"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="B378" sqref="B378"/>
+    <sheetView topLeftCell="A358" workbookViewId="0">
+      <selection activeCell="F113" sqref="F113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16601,22 +16605,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4B95C42-33DD-FC44-B810-1CFD1420D45A}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F945E9B-6912-DC4D-AE1F-6592B072C3CE}">
   <dimension ref="A1:K106"/>
   <sheetViews>
-    <sheetView topLeftCell="A84" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
       <selection activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
@@ -20344,7 +20336,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C143FBD-A206-B544-9666-5498B5D2D990}">
   <dimension ref="A1:D17"/>
   <sheetViews>
@@ -20597,11 +20589,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F341486-F420-B446-936A-48CE3BB4D74B}">
   <dimension ref="A1:E106"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A88" workbookViewId="0">
       <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
@@ -21478,7 +21470,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF517485-00F5-6F49-972F-5CDEEB391FEF}">
   <dimension ref="A1:G373"/>
   <sheetViews>

</xml_diff>